<commit_message>
EU27 Updated io-model/HSR, switched to 2019 Q3-4 averaged savings rate to avoid pandemic-inflated values.
</commit_message>
<xml_diff>
--- a/InputData/io-model/HSR/Household Savings Rate.xlsx
+++ b/InputData/io-model/HSR/Household Savings Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adolg\Dropbox\Energy Innovation IO\Deliverable IO files\EU\HSR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\eps-eu\InputData\io-model\HSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAB27FB-8974-47FF-BC01-FF65500A5087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB40640B-1030-4239-8793-1791644BBF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="24195" windowHeight="20145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29865" yWindow="2445" windowWidth="22545" windowHeight="12780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -76,16 +76,16 @@
     <t>https://ec.europa.eu/eurostat/databrowser/view/teina500/default/table?lang=en</t>
   </si>
   <si>
-    <t>2020-Q3 savings rate for EU28</t>
-  </si>
-  <si>
-    <t>We use data for Q3-2020 in part because the household savings</t>
-  </si>
-  <si>
     <t>rate spiked after the start of the coronavirus pandemic; we do not</t>
   </si>
   <si>
     <t>expect savings to remain as high as they have been recently.</t>
+  </si>
+  <si>
+    <t>2019-Q3/4 savings rate for EU27</t>
+  </si>
+  <si>
+    <t>We average data from Q3/4-2019 in part because the household savings</t>
   </si>
 </sst>
 </file>
@@ -478,18 +478,18 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -497,69 +497,69 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -578,27 +578,27 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5">
-        <f>0.0997</f>
-        <v>9.9699999999999997E-2</v>
+        <f>AVERAGE(0.1197,0.1249)</f>
+        <v>0.12229999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>